<commit_message>
YOR-18 update import mechanism to support attributes for phase one
</commit_message>
<xml_diff>
--- a/importer/src/test/resources/testdata/right_column_order.xlsx
+++ b/importer/src/test/resources/testdata/right_column_order.xlsx
@@ -15,21 +15,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>tone</t>
-  </si>
-  <si>
-    <t>meaning</t>
-  </si>
-  <si>
-    <t>morphology</t>
-  </si>
-  <si>
-    <t>location</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Pronunciation</t>
+  </si>
+  <si>
+    <t>IPA_notation</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t>Syllable</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Extended_Meaning</t>
+  </si>
+  <si>
+    <t>Morphology</t>
+  </si>
+  <si>
+    <t>Etymology</t>
+  </si>
+  <si>
+    <t>Geo_location</t>
+  </si>
+  <si>
+    <t>Media</t>
   </si>
   <si>
     <t>Kola</t>
@@ -75,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -105,13 +123,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -192,7 +203,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,7 +211,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,7 +219,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -309,10 +320,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:340"/>
+  <dimension ref="A1:N340"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -330,10 +341,10 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -342,49 +353,66 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,6 +1424,12 @@
       <c r="A340" s="5"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J1" type="list">
+      <formula1>"ABEOKUTA,AKURE,IBADAN,EKO,IGBOMINA,YAGBA,ILESHA,IFE,EKITI,AKURE,EFON,OKITIPUPA,IJALE,ONDO,OWO,IKARE,SAGAMU,,OKITIPUPA"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>